<commit_message>
QA Renew By Richard 20160107
</commit_message>
<xml_diff>
--- a/02_Management/OZtuantuan_QA.xlsx
+++ b/02_Management/OZtuantuan_QA.xlsx
@@ -4,19 +4,99 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="19395" windowHeight="7605"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575"/>
   </bookViews>
   <sheets>
-    <sheet name="20160106" sheetId="1" r:id="rId1"/>
+    <sheet name="QA" sheetId="3" r:id="rId1"/>
+    <sheet name="20160106" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Q1:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+  <si>
+    <t>关于Checkout，你们希望有几个步骤？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般建议：是否注册-&gt;邮寄地址-&gt;发票信息-&gt;运送方式-&gt;付款方式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>看看是否都需要？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>另外，关于邮寄地址，是否让客户保留几个常用的选择？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>还有，发票信息的话，需要填什么，是不是每次都填？麻烦提供一下。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>看一下：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>metronic_v3.0.2/metronic_v2.0.2/ecommerce/template/checkout.html</t>
+  </si>
+  <si>
+    <t>看看你们想怎么考虑？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于基础数据，能早点提供的话更好，这样我们这边开发和调试的话会比较直观。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于登陆，是不是考虑手机号或者邮箱都可以作为用户名去登陆？就不考虑什么登陆ID了吧？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>短信服务商OK的话，是否可以让我们先接入试试？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Question</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Answer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q By</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A By</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A Date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q Date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>QA About Oztuantuan</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -24,46 +104,82 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Q2：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>我目前的设想是一个商品最起码要4张图片。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q3：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>关于Checkout，你们希望有几个步骤？</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>一般建议：是否注册-&gt;邮寄地址-&gt;发票信息-&gt;运送方式-&gt;付款方式</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>看看是否都需要？</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>另外，关于邮寄地址，是否让客户保留几个常用的选择？</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>还有，发票信息的话，需要填什么，是不是每次都填？麻烦提供一下。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>看一下：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>metronic_v3.0.2/metronic_v2.0.2/ecommerce/template/checkout.html</t>
-  </si>
-  <si>
-    <t>看看你们想怎么考虑？</t>
+    <t>Richard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以的，尽快提供图片。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Close</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于Logo，是否可以提供一下？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016/1/7提供的素材无法使用。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于首页设计：
+1)横向导航栏怎么设计？
+2)四幅广告图怎么考虑？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet【20160106】</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>未回答</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2)用Slide方式实现四幅广告图，后期考虑后台可以维护。</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于Checkout的步骤和内容，需要明确一下。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以的，尽快提供。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -71,23 +187,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>关于基础数据，能早点提供的话更好，这样我们这边开发和调试的话会比较直观。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q5：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>关于登陆，是不是考虑手机号或者邮箱都可以作为用户名去登陆？就不考虑什么登陆ID了吧？</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q6：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>短信服务商OK的话，是否可以让我们先接入试试？</t>
+    <t>可以的，已邮件提供相关信息。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不需要登陆ID，用手机号/邮箱/微信号登陆，如果是邮箱或者微信号的话，必须要绑定手机。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于商品团购页面的Tab内容：目前我设计的是三个（本单详情、消费提示、商家规则），看提供的原来的网站设计稿的话，还不止，不知你们是怎么考虑的。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -95,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,16 +236,45 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,13 +282,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -159,6 +311,51 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -181,13 +378,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>15241</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -219,13 +416,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -279,13 +476,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
       <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -344,13 +541,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -404,13 +601,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -464,13 +661,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -550,13 +747,13 @@
     <xdr:from>
       <xdr:col>44</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -620,13 +817,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>89697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -974,106 +1171,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="14">
+        <v>42375</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="14">
+        <v>42376</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <f>A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42375</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <f t="shared" ref="A5:A10" si="0">A4+1</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7">
+        <v>42375</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7">
+        <v>42376</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7">
+        <v>42375</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>42375</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7">
+        <v>42376</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="14">
+        <v>42375</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="14">
+        <v>42376</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14">
+        <v>42375</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="14">
+        <v>42376</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42376</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T41"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B2" s="1" t="s">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B3" s="1" t="s">
+      <c r="T35" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="T36" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="T37" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="B37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="T38" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T39" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="T40" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T41" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="T42" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="T43" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B54" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B57" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B60" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QA renew By Richard 20160112
</commit_message>
<xml_diff>
--- a/02_Management/OZtuantuan_QA.xlsx
+++ b/02_Management/OZtuantuan_QA.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16580"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="3" r:id="rId1"/>
     <sheet name="20160106" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>关于Checkout，你们希望有几个步骤？</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -142,60 +147,40 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>未回答</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>关于Checkout的步骤和内容，需要明确一下。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以的，尽快提供。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q4：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以的，已邮件提供相关信息。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不需要登陆ID，用手机号/邮箱/微信号登陆，如果是邮箱或者微信号的话，必须要绑定手机。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于商品团购页面的Tab内容：目前我设计的是三个（本单详情、消费提示、商家规则），看提供的原来的网站设计稿的话，还不止，不知你们是怎么考虑的。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1)团购、求购、热门、零售
 2)用Slide方式实现四幅广告图，后期考虑后台可以维护。</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>关于Checkout的步骤和内容，需要明确一下。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以的，尽快提供。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q4：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以的，已邮件提供相关信息。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不需要登陆ID，用手机号/邮箱/微信号登陆，如果是邮箱或者微信号的话，必须要绑定手机。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>关于商品团购页面的Tab内容：目前我设计的是三个（本单详情、消费提示、商家规则），看提供的原来的网站设计稿的话，还不止，不知你们是怎么考虑的。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>已提供，但大小像素是否合适正在确认中。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -203,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,16 +230,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +250,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -284,16 +267,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -303,7 +286,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -358,9 +341,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1173,26 +1159,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="42.875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.83203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1221,7 +1209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="36" customHeight="1">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1248,7 +1236,7 @@
       </c>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="36" customHeight="1">
       <c r="A4" s="5">
         <f>A3+1</f>
         <v>2</v>
@@ -1262,7 +1250,9 @@
       <c r="D4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
@@ -1272,7 +1262,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="36" customHeight="1">
       <c r="A5" s="5">
         <f t="shared" ref="A5:A10" si="0">A4+1</f>
         <v>3</v>
@@ -1287,7 +1277,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F5" s="7">
         <v>42376</v>
@@ -1302,13 +1292,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="36" customHeight="1">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7">
         <v>42375</v>
@@ -1326,7 +1316,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="36" customHeight="1">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1341,7 +1331,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7">
         <v>42376</v>
@@ -1354,7 +1344,7 @@
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="36" customHeight="1">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1369,7 +1359,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="14">
         <v>42376</v>
@@ -1382,7 +1372,7 @@
       </c>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="36" customHeight="1">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1397,7 +1387,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="14">
         <v>42376</v>
@@ -1410,13 +1400,13 @@
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="36" customHeight="1">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="7">
         <v>42376</v>
@@ -1432,14 +1422,19 @@
       </c>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:9" ht="36" customHeight="1"/>
+    <row r="12" spans="1:9" ht="36" customHeight="1"/>
+    <row r="13" spans="1:9" ht="36" customHeight="1"/>
+    <row r="14" spans="1:9" ht="36" customHeight="1"/>
+    <row r="15" spans="1:9" ht="36" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1447,32 +1442,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20">
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1480,27 +1475,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20">
       <c r="T36" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20">
       <c r="T37" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20">
       <c r="T39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20">
       <c r="T40" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20">
       <c r="T41" s="1" t="s">
         <v>7</v>
       </c>
@@ -1509,5 +1504,10 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QA renew By Richard 20160113
</commit_message>
<xml_diff>
--- a/02_Management/OZtuantuan_QA.xlsx
+++ b/02_Management/OZtuantuan_QA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16580"/>
+    <workbookView xWindow="2000" yWindow="180" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>关于Checkout，你们希望有几个步骤？</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -181,6 +181,30 @@
   </si>
   <si>
     <t>已提供，但大小像素是否合适正在确认中。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在checkout时，会自动根据购买的商品和用户的信息生成invoice,约定是PDF格式，那么希望能提供一个生成格式。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>invoice生成后需要发送到用户的邮箱去，那么对于用手机号注册的用户，是不是在checkout的时候要提示客户先输入一个邮箱？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择普通快递的时候，填写地址相关信息，是不是只需要填写：收货人、收货地址、邮编、联系方式等就OK？这些地址是否需要保存为用户的常用地址供其下次购买时选择？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>已提供。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lan</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -188,7 +212,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +251,24 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -281,8 +323,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -345,7 +435,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,9 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -1263,86 +1367,92 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1">
-      <c r="A5" s="5">
-        <f t="shared" ref="A5:A10" si="0">A4+1</f>
+      <c r="A5" s="12">
+        <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="14">
         <v>42375</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="14">
         <v>42376</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="9" t="s">
+      <c r="H5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1">
-      <c r="A6" s="5">
+      <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="14">
         <v>42375</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="E6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="14">
+        <v>42381</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1">
-      <c r="A7" s="5">
+      <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="14">
         <v>42375</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="14">
         <v>42376</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="9"/>
+      <c r="G7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="36" customHeight="1">
       <c r="A8" s="12">
@@ -1393,7 +1503,7 @@
         <v>42376</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>25</v>
@@ -1422,14 +1532,78 @@
       </c>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" ht="36" customHeight="1"/>
-    <row r="12" spans="1:9" ht="36" customHeight="1"/>
-    <row r="13" spans="1:9" ht="36" customHeight="1"/>
+    <row r="11" spans="1:9" ht="36" customHeight="1">
+      <c r="A11" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7">
+        <v>42382</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="36" customHeight="1">
+      <c r="A12" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="7">
+        <v>42382</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="36" customHeight="1">
+      <c r="A13" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7">
+        <v>42382</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="11"/>
+    </row>
     <row r="14" spans="1:9" ht="36" customHeight="1"/>
     <row r="15" spans="1:9" ht="36" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
QA renew By Richard 20160114
</commit_message>
<xml_diff>
--- a/02_Management/OZtuantuan_QA.xlsx
+++ b/02_Management/OZtuantuan_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="180" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1995" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="3" r:id="rId1"/>
     <sheet name="20160106" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>关于Checkout，你们希望有几个步骤？</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,10 +130,6 @@
   </si>
   <si>
     <t>关于Logo，是否可以提供一下？</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016/1/7提供的素材无法使用。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -180,10 +176,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>已提供，但大小像素是否合适正在确认中。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>在checkout时，会自动根据购买的商品和用户的信息生成invoice,约定是PDF格式，那么希望能提供一个生成格式。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -202,6 +194,28 @@
   <si>
     <t>Lan</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要填写，手机注册的用户注册后最好要强制完善个人信息，邮箱要填上去。或者按你说的在发invoice的时候填写。</t>
+  </si>
+  <si>
+    <t>这个我们会提供的</t>
+  </si>
+  <si>
+    <t>就按照商品详情、消费提示、商家规则三个tab就好</t>
+  </si>
+  <si>
+    <t>2016/1/7提供的素材无法使用。</t>
+  </si>
+  <si>
+    <t>已提供，但大小像素是否合适正在确认中。提供的是AI文件，大小可以任意调整</t>
+  </si>
+  <si>
+    <t>需要，并且应该有一个能自动计算运费的功能，这个澳大利亚邮局有api可以使用。货到付款的方式，我们自己有一个列表，里面列出了不同的社区不同的收费价格表，货到付款填写地址时 suburb是一个下拉菜单，只能在其中选择，其他的地方我们是不送的，对应的价格有一个excel表，到时一并发你</t>
   </si>
   <si>
     <t>Lan</t>
@@ -436,6 +450,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="17">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -444,18 +459,45 @@
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1263,28 +1305,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.83203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="42.83203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="42.875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.625" style="4" customWidth="1"/>
     <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="10" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1313,7 +1355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="36" customHeight="1">
+    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1340,7 +1382,7 @@
       </c>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="36" customHeight="1">
+    <row r="4" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <f>A3+1</f>
         <v>2</v>
@@ -1355,7 +1397,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
@@ -1363,16 +1405,16 @@
         <v>26</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="36" customHeight="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="36" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="14">
         <v>42375</v>
@@ -1381,7 +1423,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="14">
         <v>42376</v>
@@ -1393,16 +1435,16 @@
         <v>25</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="36" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="14">
         <v>42375</v>
@@ -1411,22 +1453,22 @@
         <v>22</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="14">
         <v>42381</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="36" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1441,20 +1483,20 @@
         <v>22</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="14">
         <v>42376</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" ht="36" customHeight="1">
+    <row r="8" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1469,7 +1511,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="14">
         <v>42376</v>
@@ -1482,7 +1524,7 @@
       </c>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="1:9" ht="36" customHeight="1">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1497,26 +1539,26 @@
         <v>22</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="14">
         <v>42376</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>25</v>
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="36" customHeight="1">
+    <row r="10" spans="1:9" ht="36" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7">
         <v>42376</v>
@@ -1524,21 +1566,27 @@
       <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+      <c r="E10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="7">
+        <v>42383</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:9" ht="36" customHeight="1">
+    <row r="11" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="7">
         <v>42382</v>
@@ -1546,21 +1594,27 @@
       <c r="D11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="7">
+        <v>42383</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:9" ht="36" customHeight="1">
+    <row r="12" spans="1:9" ht="36" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7">
         <v>42382</v>
@@ -1568,21 +1622,27 @@
       <c r="D12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="E12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="7">
+        <v>42383</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" spans="1:9" ht="36" customHeight="1">
+    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="7">
         <v>42382</v>
@@ -1590,25 +1650,24 @@
       <c r="D13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="7">
+        <v>42383</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" ht="36" customHeight="1"/>
-    <row r="15" spans="1:9" ht="36" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1618,30 +1677,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="33" spans="1:20">
-      <c r="A33" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1649,27 +1708,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T36" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T37" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T40" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="T41" s="1" t="s">
         <v>7</v>
       </c>
@@ -1678,10 +1737,5 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>